<commit_message>
se agraga excel con etiqueta
</commit_message>
<xml_diff>
--- a/Exportaciones-agrícolas-no-tradicionales-y-tradicionales.xlsx
+++ b/Exportaciones-agrícolas-no-tradicionales-y-tradicionales.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alzat\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alzat\OneDrive\Documentos\Desafio1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82091C0-7291-4F3C-ACB0-758581F4DF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6619835-C378-49D5-9A66-5BDC4464EACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$M$1</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -509,7 +512,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B347" sqref="B347"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6916,6 +6919,7 @@
       <c r="M345" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>